<commit_message>
create import student funtion
</commit_message>
<xml_diff>
--- a/data/学生库.xlsx
+++ b/data/学生库.xlsx
@@ -1,47 +1,135 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyScan\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>data1</t>
-  </si>
-  <si>
-    <t>data2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+  <si>
+    <t>班级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高三一班</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王大宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+  </si>
+  <si>
+    <t>李晓燕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李梅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王强</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张刚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>傅园慧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周家宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈宝强</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唐建业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纪晓岚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王刚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张小二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>于小慧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金善宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唐兰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -57,15 +145,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -355,196 +456,252 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A2:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="175" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
-        <v>100</v>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>40</v>
-      </c>
-      <c r="C5" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="n">
-        <v>40</v>
-      </c>
-      <c r="C6" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" t="n">
-        <v>50</v>
-      </c>
-      <c r="C7" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="n">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B8" t="n">
-        <v>30</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" t="n">
-        <v>25</v>
-      </c>
-      <c r="C9" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="n">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B10" t="n">
-        <v>50</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>40</v>
-      </c>
-      <c r="C12" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="n">
-        <v>40</v>
-      </c>
-      <c r="C13" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="n">
-        <v>4</v>
-      </c>
-      <c r="B14" t="n">
-        <v>50</v>
-      </c>
-      <c r="C14" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="n">
-        <v>5</v>
-      </c>
-      <c r="B15" t="n">
-        <v>30</v>
-      </c>
-      <c r="C15" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" t="n">
-        <v>25</v>
-      </c>
-      <c r="C16" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="n">
-        <v>7</v>
-      </c>
-      <c r="B17" t="n">
-        <v>50</v>
-      </c>
-      <c r="C17" t="n">
-        <v>10</v>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="STwWuaUk8tjbHlERroIDNwTIQrzMCHenfcGIQYvGv51eUTiGeAW8sMxnIr0IhjtSxM6RX1VzuSUpPcvAFO9k3w==" saltValue="ezqkBTuqhcUALbFGkXnJbQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>"男,女"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>